<commit_message>
[VM:timothy.queen@7/17/2014 8:56:00 AM] added risk
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13645
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
+++ b/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="65">
   <si>
     <t>Status</t>
   </si>
@@ -212,6 +212,18 @@
   </si>
   <si>
     <t>Risk is closed</t>
+  </si>
+  <si>
+    <t>Lack of hierarchy information - supervisor--&gt; manager--&gt; sr. manager in peoplesoft feed</t>
+  </si>
+  <si>
+    <t>Suzy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCO Operations  </t>
+  </si>
+  <si>
+    <t>Lack of hierarchy information in data feed for supervisors, managers, sr managers will prevent the proper escalation of eCL issues for Supervisors</t>
   </si>
 </sst>
 </file>
@@ -1405,8 +1417,8 @@
   </sheetPr>
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="K2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1421,7 +1433,7 @@
     <col min="8" max="8" width="12.5546875" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" customWidth="1"/>
     <col min="12" max="12" width="10.6640625" customWidth="1"/>
     <col min="13" max="13" width="9.109375" customWidth="1"/>
     <col min="14" max="14" width="11.44140625" customWidth="1"/>
@@ -1913,29 +1925,43 @@
       </c>
       <c r="U9" s="9"/>
     </row>
-    <row r="10" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
+    <row r="10" spans="1:21" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="9">
+        <v>41837</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>21</v>
+      <c r="G10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="K10" s="19">
+        <v>5</v>
       </c>
       <c r="L10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
+      <c r="M10" s="20">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>18.75</v>
       </c>
       <c r="N10" s="11" t="e">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
@@ -1955,7 +1981,6 @@
       <c r="B11" s="8"/>
       <c r="C11" s="4"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="5"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -2955,7 +2980,7 @@
     <mergeCell ref="A2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="17" scale="39" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="17" scale="38" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;LVangent Proprietary Information</oddFooter>
   </headerFooter>
@@ -2966,18 +2991,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3095,6 +3120,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -3105,14 +3138,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[VM:timothy.queen@8/1/2014 12:54:44 PM] updates made
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13674
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
+++ b/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="70">
   <si>
     <t>Status</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Incomplete and inaccurate data in centrallized CCO CSR/Employee database</t>
   </si>
   <si>
-    <t>Changes, such as changes to quality monitoring tools may impact functionality and reuire engineering changes</t>
-  </si>
-  <si>
     <t>Utilizing LimeSurvey and Verint; new scorecard and scoring system</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
     <t>Opportunities for improvement will be investigated; hardware changes may be needed</t>
   </si>
   <si>
-    <t>Users are not able to perform their job</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -224,6 +218,28 @@
   </si>
   <si>
     <t>Lack of hierarchy information in data feed for supervisors, managers, sr managers will prevent the proper escalation of eCL issues for Supervisors</t>
+  </si>
+  <si>
+    <t>Changes, such as changes to quality monitoring tools may impact functionality and require engineering changes</t>
+  </si>
+  <si>
+    <t>Users are not able to perform their job
+Risk is Closed 7/30/14</t>
+  </si>
+  <si>
+    <t>Engineers supporting multiple projects will have negative impact on delivery of eCL changes</t>
+  </si>
+  <si>
+    <t>Resources are supporting eCL, Performance Scorecard, A&amp;E, IQS, Aspect</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>eCL team</t>
+  </si>
+  <si>
+    <t>Balance work load across engineers to the greatest extent possible to prevent distractions.</t>
   </si>
 </sst>
 </file>
@@ -801,7 +817,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -866,9 +882,6 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -886,6 +899,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -935,6 +954,32 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="22">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -987,32 +1032,6 @@
       </font>
       <numFmt numFmtId="5" formatCode="#,##0_);\(#,##0\)"/>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1104,22 +1123,22 @@
     <tableColumn id="6" uniqueName="Owner" name="Risk Owner" queryTableFieldId="5" dataDxfId="15"/>
     <tableColumn id="7" uniqueName="Origin" name="Origin" queryTableFieldId="6" dataDxfId="14"/>
     <tableColumn id="8" uniqueName="Stakeholders" name="Stakeholders" queryTableFieldId="7" dataDxfId="13"/>
-    <tableColumn id="9" uniqueName="Category" name="Category" queryTableFieldId="8" dataDxfId="12"/>
-    <tableColumn id="10" uniqueName="Probability" name="Probability of Occurrence (%) " queryTableFieldId="9" dataDxfId="11" dataCellStyle="Percent"/>
-    <tableColumn id="11" uniqueName="Impact" name="Impact  _x000a_Rating   (1-5)" queryTableFieldId="10" dataDxfId="10" dataCellStyle="Currency"/>
-    <tableColumn id="21" uniqueName="21" name="Total Impact on occurance_x000a_$" queryTableFieldId="26" dataDxfId="9" dataCellStyle="Currency"/>
-    <tableColumn id="12" uniqueName="Risk_x005f_x0020_Exposure" name="Risk Exposure Ranking_x000a_(1 - 25)" queryTableFieldId="11" dataDxfId="8"/>
-    <tableColumn id="13" uniqueName="13" name="Risk Exposure Estimate   ($)" queryTableFieldId="24" dataDxfId="7">
+    <tableColumn id="9" uniqueName="Category" name="Category" queryTableFieldId="8" dataDxfId="2"/>
+    <tableColumn id="10" uniqueName="Probability" name="Probability of Occurrence (%) " queryTableFieldId="9" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="11" uniqueName="Impact" name="Impact  _x000a_Rating   (1-5)" queryTableFieldId="10" dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="21" uniqueName="21" name="Total Impact on occurance_x000a_$" queryTableFieldId="26" dataDxfId="12" dataCellStyle="Currency"/>
+    <tableColumn id="12" uniqueName="Risk_x005f_x0020_Exposure" name="Risk Exposure Ranking_x000a_(1 - 25)" queryTableFieldId="11" dataDxfId="11"/>
+    <tableColumn id="13" uniqueName="13" name="Risk Exposure Estimate   ($)" queryTableFieldId="24" dataDxfId="10">
       <calculatedColumnFormula>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
 $]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" uniqueName="20" name="Basis of Risk Exposure Estimate" queryTableFieldId="25" dataDxfId="6"/>
-    <tableColumn id="14" uniqueName="Mitigation_x005f_x0020_Plan" name="Mitigation Plan" queryTableFieldId="13" dataDxfId="5"/>
-    <tableColumn id="15" uniqueName="Mitigation_x005f_x0020_Start_x005f_x0020_Dat" name="Mitigation Start Date" queryTableFieldId="14" dataDxfId="4"/>
-    <tableColumn id="16" uniqueName="Mitigation_x005f_x0020_Stop_x005f_x0020_Date" name="Mitigation Stop Date" queryTableFieldId="15" dataDxfId="3"/>
-    <tableColumn id="17" uniqueName="Contingency_x005f_x0020_Plan" name="Contingency Plan" queryTableFieldId="16" dataDxfId="2"/>
-    <tableColumn id="18" uniqueName="Threshold_x005f_x002f_Trigger" name="Threshold/ Trigger" queryTableFieldId="17" dataDxfId="1"/>
-    <tableColumn id="19" uniqueName="Contingency_x005f_x0020_Start_x005f_x0020_Da" name="Contingency Start Date" queryTableFieldId="18" dataDxfId="0"/>
+    <tableColumn id="20" uniqueName="20" name="Basis of Risk Exposure Estimate" queryTableFieldId="25" dataDxfId="9"/>
+    <tableColumn id="14" uniqueName="Mitigation_x005f_x0020_Plan" name="Mitigation Plan" queryTableFieldId="13" dataDxfId="8"/>
+    <tableColumn id="15" uniqueName="Mitigation_x005f_x0020_Start_x005f_x0020_Dat" name="Mitigation Start Date" queryTableFieldId="14" dataDxfId="7"/>
+    <tableColumn id="16" uniqueName="Mitigation_x005f_x0020_Stop_x005f_x0020_Date" name="Mitigation Stop Date" queryTableFieldId="15" dataDxfId="6"/>
+    <tableColumn id="17" uniqueName="Contingency_x005f_x0020_Plan" name="Contingency Plan" queryTableFieldId="16" dataDxfId="5"/>
+    <tableColumn id="18" uniqueName="Threshold_x005f_x002f_Trigger" name="Threshold/ Trigger" queryTableFieldId="17" dataDxfId="4"/>
+    <tableColumn id="19" uniqueName="Contingency_x005f_x0020_Start_x005f_x0020_Da" name="Contingency Start Date" queryTableFieldId="18" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1418,7 +1437,7 @@
   <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1447,54 +1466,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="24" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="25"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="24"/>
     </row>
     <row r="2" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="28"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="27"/>
     </row>
     <row r="3" spans="1:21" ht="58.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1587,7 +1606,7 @@
       <c r="I4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="28">
         <v>1</v>
       </c>
       <c r="K4" s="19">
@@ -1615,7 +1634,7 @@
       </c>
       <c r="R4" s="7"/>
       <c r="S4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T4" s="8" t="s">
         <v>31</v>
@@ -1624,7 +1643,7 @@
     </row>
     <row r="5" spans="1:21" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="4" t="s">
@@ -1634,7 +1653,7 @@
         <v>41013</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>33</v>
@@ -1648,7 +1667,7 @@
       <c r="I5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="28">
         <v>1</v>
       </c>
       <c r="K5" s="19">
@@ -1674,10 +1693,10 @@
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
       <c r="S5" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="U5" s="7"/>
     </row>
@@ -1707,7 +1726,7 @@
       <c r="I6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="28">
         <v>1</v>
       </c>
       <c r="K6" s="19">
@@ -1728,33 +1747,33 @@
       </c>
       <c r="O6" s="12"/>
       <c r="P6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q6" s="7">
         <v>41731</v>
       </c>
       <c r="R6" s="7"/>
       <c r="S6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="T6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="T6" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="U6" s="7"/>
     </row>
-    <row r="7" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="4" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D7" s="9">
         <v>41414</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>33</v>
@@ -1768,7 +1787,7 @@
       <c r="I7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="28">
         <v>1</v>
       </c>
       <c r="K7" s="19">
@@ -1789,17 +1808,17 @@
       </c>
       <c r="O7" s="13"/>
       <c r="P7" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q7" s="9">
         <v>41760</v>
       </c>
       <c r="R7" s="9"/>
       <c r="S7" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U7" s="9"/>
     </row>
@@ -1809,13 +1828,13 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="9">
         <v>41438</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>33</v>
@@ -1829,7 +1848,7 @@
       <c r="I8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="28">
         <v>1</v>
       </c>
       <c r="K8" s="19">
@@ -1850,33 +1869,33 @@
       </c>
       <c r="O8" s="14"/>
       <c r="P8" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q8" s="9">
         <v>41791</v>
       </c>
       <c r="R8" s="9"/>
       <c r="S8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="T8" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="T8" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="U8" s="9"/>
     </row>
-    <row r="9" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9">
         <v>41619</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>33</v>
@@ -1890,7 +1909,7 @@
       <c r="I9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="28">
         <v>0.25</v>
       </c>
       <c r="K9" s="19">
@@ -1911,17 +1930,19 @@
       </c>
       <c r="O9" s="15"/>
       <c r="P9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q9" s="9">
         <v>41803</v>
       </c>
-      <c r="R9" s="9"/>
+      <c r="R9" s="9">
+        <v>41850</v>
+      </c>
       <c r="S9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="U9" s="9"/>
     </row>
@@ -1931,25 +1952,25 @@
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D10" s="9">
         <v>41837</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="28">
         <v>0.75</v>
       </c>
       <c r="K10" s="19">
@@ -1976,28 +1997,45 @@
       <c r="T10" s="8"/>
       <c r="U10" s="9"/>
     </row>
-    <row r="11" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
+    <row r="11" spans="1:21" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="9"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>21</v>
+      <c r="C11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="9">
+        <v>41850</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="28">
+        <v>0.85</v>
+      </c>
+      <c r="K11" s="19">
+        <v>5</v>
       </c>
       <c r="L11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="M11" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
+      <c r="M11" s="20">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>21.25</v>
       </c>
       <c r="N11" s="11" t="e">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
@@ -2005,10 +2043,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="O11" s="15"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="9"/>
+      <c r="P11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>41850</v>
+      </c>
       <c r="R11" s="9"/>
-      <c r="S11" s="5"/>
+      <c r="S11" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="T11" s="8"/>
       <c r="U11" s="9"/>
     </row>
@@ -2022,7 +2066,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K12" s="19" t="s">
@@ -2059,7 +2103,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K13" s="19" t="s">
@@ -2096,7 +2140,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="22" t="s">
+      <c r="J14" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K14" s="19" t="s">
@@ -2133,7 +2177,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="22" t="s">
+      <c r="J15" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K15" s="19" t="s">
@@ -2170,7 +2214,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="22" t="s">
+      <c r="J16" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K16" s="19" t="s">
@@ -2207,7 +2251,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="8"/>
-      <c r="J17" s="22" t="s">
+      <c r="J17" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K17" s="19" t="s">
@@ -2244,7 +2288,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="8"/>
-      <c r="J18" s="22" t="s">
+      <c r="J18" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K18" s="19" t="s">
@@ -2281,7 +2325,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="8"/>
-      <c r="J19" s="22" t="s">
+      <c r="J19" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K19" s="19" t="s">
@@ -2318,7 +2362,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="8"/>
-      <c r="J20" s="22" t="s">
+      <c r="J20" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K20" s="19" t="s">
@@ -2355,7 +2399,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="22" t="s">
+      <c r="J21" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K21" s="19" t="s">
@@ -2392,7 +2436,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="22" t="s">
+      <c r="J22" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K22" s="19" t="s">
@@ -2429,7 +2473,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="22" t="s">
+      <c r="J23" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K23" s="19" t="s">
@@ -2466,7 +2510,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="22" t="s">
+      <c r="J24" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K24" s="19" t="s">
@@ -2503,7 +2547,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="8"/>
-      <c r="J25" s="22" t="s">
+      <c r="J25" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K25" s="19" t="s">
@@ -2540,7 +2584,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="8"/>
-      <c r="J26" s="22" t="s">
+      <c r="J26" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K26" s="19" t="s">
@@ -2577,7 +2621,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="8"/>
-      <c r="J27" s="22" t="s">
+      <c r="J27" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K27" s="19" t="s">
@@ -2614,7 +2658,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="8"/>
-      <c r="J28" s="22" t="s">
+      <c r="J28" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K28" s="19" t="s">
@@ -2651,7 +2695,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="8"/>
-      <c r="J29" s="22" t="s">
+      <c r="J29" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K29" s="19" t="s">
@@ -2688,7 +2732,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="8"/>
-      <c r="J30" s="22" t="s">
+      <c r="J30" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K30" s="19" t="s">
@@ -2725,7 +2769,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="8"/>
-      <c r="J31" s="22" t="s">
+      <c r="J31" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K31" s="19" t="s">
@@ -2762,7 +2806,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="8"/>
-      <c r="J32" s="22" t="s">
+      <c r="J32" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K32" s="19" t="s">
@@ -2799,7 +2843,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="8"/>
-      <c r="J33" s="22" t="s">
+      <c r="J33" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K33" s="19" t="s">
@@ -2836,7 +2880,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="8"/>
-      <c r="J34" s="22" t="s">
+      <c r="J34" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K34" s="19" t="s">
@@ -2873,7 +2917,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="8"/>
-      <c r="J35" s="22" t="s">
+      <c r="J35" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K35" s="19" t="s">
@@ -2910,7 +2954,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="8"/>
-      <c r="J36" s="22" t="s">
+      <c r="J36" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K36" s="19" t="s">
@@ -2947,7 +2991,7 @@
       <c r="G37" s="4"/>
       <c r="H37" s="5"/>
       <c r="I37" s="8"/>
-      <c r="J37" s="22" t="s">
+      <c r="J37" s="28" t="s">
         <v>21</v>
       </c>
       <c r="K37" s="19" t="s">
@@ -2991,18 +3035,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3120,14 +3164,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -3138,6 +3174,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[VM:timothy.queen@2/23/2015 3:01:14 PM] updated 2/23/15
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13964
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
+++ b/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="132" windowWidth="13392" windowHeight="7488"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="Integrated Register" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="owssvr_2" localSheetId="0" hidden="1">'Integrated Register'!$A$3:$U$37</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Integrated Register'!$A$1:$U$37</definedName>
+    <definedName name="owssvr_2" localSheetId="0" hidden="1">'Integrated Register'!$A$3:$V$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Integrated Register'!$A$1:$V$37</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="72">
   <si>
     <t>Status</t>
   </si>
@@ -187,9 +187,6 @@
     <t>User reports inaccurate data in the eCL</t>
   </si>
   <si>
-    <t>Monitoring system changes</t>
-  </si>
-  <si>
     <t>System will be updated as needed</t>
   </si>
   <si>
@@ -230,9 +227,6 @@
     <t>Engineers supporting multiple projects will have negative impact on delivery of eCL changes</t>
   </si>
   <si>
-    <t>Resources are supporting eCL, Performance Scorecard, A&amp;E, IQS, Aspect</t>
-  </si>
-  <si>
     <t>Tim</t>
   </si>
   <si>
@@ -240,6 +234,18 @@
   </si>
   <si>
     <t>Balance work load across engineers to the greatest extent possible to prevent distractions.</t>
+  </si>
+  <si>
+    <t>Closed 2/23/15 - hierarchy information is in the peoplesoft file</t>
+  </si>
+  <si>
+    <t>Date Modified</t>
+  </si>
+  <si>
+    <t>Resources are supporting eCL, Performance Scorecard, A&amp;E, IQS</t>
+  </si>
+  <si>
+    <t>Monitoring system changes; Verint went into production July 1, 2014; closed 2/23/15</t>
   </si>
 </sst>
 </file>
@@ -882,6 +888,12 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -899,12 +911,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -953,32 +959,10 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="23">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
@@ -1034,6 +1018,32 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1078,12 +1088,13 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="owssvr[2]" backgroundRefresh="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="27">
-    <queryTableFields count="21">
+  <queryTableRefresh nextId="28">
+    <queryTableFields count="22">
       <queryTableField id="2" name="Status" tableColumnId="1"/>
       <queryTableField id="20" name="Project" tableColumnId="2"/>
       <queryTableField id="1" name="Description" tableColumnId="3"/>
       <queryTableField id="3" name="Date Identified" tableColumnId="4"/>
+      <queryTableField id="27" dataBound="0" tableColumnId="23"/>
       <queryTableField id="4" name="Context" tableColumnId="5"/>
       <queryTableField id="5" name="Owner" tableColumnId="6"/>
       <queryTableField id="6" name="Origin" tableColumnId="7"/>
@@ -1113,32 +1124,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_owssvr_23" displayName="Table_owssvr_23" ref="A3:U37" tableType="queryTable" totalsRowShown="0" dataDxfId="21">
-  <tableColumns count="21">
-    <tableColumn id="1" uniqueName="Status" name="Status" queryTableFieldId="2" dataDxfId="20"/>
-    <tableColumn id="2" uniqueName="Project" name="Program" queryTableFieldId="20" dataDxfId="19"/>
-    <tableColumn id="3" uniqueName="Title" name="Risk Description" queryTableFieldId="1" dataDxfId="18"/>
-    <tableColumn id="4" uniqueName="Date_x005f_x0020_Identified" name="Date Identified" queryTableFieldId="3" dataDxfId="17"/>
-    <tableColumn id="5" uniqueName="Context" name="Context" queryTableFieldId="4" dataDxfId="16"/>
-    <tableColumn id="6" uniqueName="Owner" name="Risk Owner" queryTableFieldId="5" dataDxfId="15"/>
-    <tableColumn id="7" uniqueName="Origin" name="Origin" queryTableFieldId="6" dataDxfId="14"/>
-    <tableColumn id="8" uniqueName="Stakeholders" name="Stakeholders" queryTableFieldId="7" dataDxfId="13"/>
-    <tableColumn id="9" uniqueName="Category" name="Category" queryTableFieldId="8" dataDxfId="2"/>
-    <tableColumn id="10" uniqueName="Probability" name="Probability of Occurrence (%) " queryTableFieldId="9" dataDxfId="0" dataCellStyle="Percent"/>
-    <tableColumn id="11" uniqueName="Impact" name="Impact  _x000a_Rating   (1-5)" queryTableFieldId="10" dataDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="21" uniqueName="21" name="Total Impact on occurance_x000a_$" queryTableFieldId="26" dataDxfId="12" dataCellStyle="Currency"/>
-    <tableColumn id="12" uniqueName="Risk_x005f_x0020_Exposure" name="Risk Exposure Ranking_x000a_(1 - 25)" queryTableFieldId="11" dataDxfId="11"/>
-    <tableColumn id="13" uniqueName="13" name="Risk Exposure Estimate   ($)" queryTableFieldId="24" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_owssvr_23" displayName="Table_owssvr_23" ref="A3:V37" tableType="queryTable" totalsRowShown="0" dataDxfId="22">
+  <tableColumns count="22">
+    <tableColumn id="1" uniqueName="Status" name="Status" queryTableFieldId="2" dataDxfId="21"/>
+    <tableColumn id="2" uniqueName="Project" name="Program" queryTableFieldId="20" dataDxfId="20"/>
+    <tableColumn id="3" uniqueName="Title" name="Risk Description" queryTableFieldId="1" dataDxfId="19"/>
+    <tableColumn id="4" uniqueName="Date_x005f_x0020_Identified" name="Date Identified" queryTableFieldId="3" dataDxfId="18"/>
+    <tableColumn id="23" uniqueName="23" name="Date Modified" queryTableFieldId="27" dataDxfId="0"/>
+    <tableColumn id="5" uniqueName="Context" name="Context" queryTableFieldId="4" dataDxfId="17"/>
+    <tableColumn id="6" uniqueName="Owner" name="Risk Owner" queryTableFieldId="5" dataDxfId="16"/>
+    <tableColumn id="7" uniqueName="Origin" name="Origin" queryTableFieldId="6" dataDxfId="15"/>
+    <tableColumn id="8" uniqueName="Stakeholders" name="Stakeholders" queryTableFieldId="7" dataDxfId="14"/>
+    <tableColumn id="9" uniqueName="Category" name="Category" queryTableFieldId="8" dataDxfId="13"/>
+    <tableColumn id="10" uniqueName="Probability" name="Probability of Occurrence (%) " queryTableFieldId="9" dataDxfId="12" dataCellStyle="Percent"/>
+    <tableColumn id="11" uniqueName="Impact" name="Impact  _x000a_Rating   (1-5)" queryTableFieldId="10" dataDxfId="11" dataCellStyle="Currency"/>
+    <tableColumn id="21" uniqueName="21" name="Total Impact on occurance_x000a_$" queryTableFieldId="26" dataDxfId="10" dataCellStyle="Currency"/>
+    <tableColumn id="12" uniqueName="Risk_x005f_x0020_Exposure" name="Risk Exposure Ranking_x000a_(1 - 25)" queryTableFieldId="11" dataDxfId="9"/>
+    <tableColumn id="13" uniqueName="13" name="Risk Exposure Estimate   ($)" queryTableFieldId="24" dataDxfId="8">
       <calculatedColumnFormula>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
 $]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" uniqueName="20" name="Basis of Risk Exposure Estimate" queryTableFieldId="25" dataDxfId="9"/>
-    <tableColumn id="14" uniqueName="Mitigation_x005f_x0020_Plan" name="Mitigation Plan" queryTableFieldId="13" dataDxfId="8"/>
-    <tableColumn id="15" uniqueName="Mitigation_x005f_x0020_Start_x005f_x0020_Dat" name="Mitigation Start Date" queryTableFieldId="14" dataDxfId="7"/>
-    <tableColumn id="16" uniqueName="Mitigation_x005f_x0020_Stop_x005f_x0020_Date" name="Mitigation Stop Date" queryTableFieldId="15" dataDxfId="6"/>
-    <tableColumn id="17" uniqueName="Contingency_x005f_x0020_Plan" name="Contingency Plan" queryTableFieldId="16" dataDxfId="5"/>
-    <tableColumn id="18" uniqueName="Threshold_x005f_x002f_Trigger" name="Threshold/ Trigger" queryTableFieldId="17" dataDxfId="4"/>
-    <tableColumn id="19" uniqueName="Contingency_x005f_x0020_Start_x005f_x0020_Da" name="Contingency Start Date" queryTableFieldId="18" dataDxfId="3"/>
+    <tableColumn id="20" uniqueName="20" name="Basis of Risk Exposure Estimate" queryTableFieldId="25" dataDxfId="7"/>
+    <tableColumn id="14" uniqueName="Mitigation_x005f_x0020_Plan" name="Mitigation Plan" queryTableFieldId="13" dataDxfId="6"/>
+    <tableColumn id="15" uniqueName="Mitigation_x005f_x0020_Start_x005f_x0020_Dat" name="Mitigation Start Date" queryTableFieldId="14" dataDxfId="5"/>
+    <tableColumn id="16" uniqueName="Mitigation_x005f_x0020_Stop_x005f_x0020_Date" name="Mitigation Stop Date" queryTableFieldId="15" dataDxfId="4"/>
+    <tableColumn id="17" uniqueName="Contingency_x005f_x0020_Plan" name="Contingency Plan" queryTableFieldId="16" dataDxfId="3"/>
+    <tableColumn id="18" uniqueName="Threshold_x005f_x002f_Trigger" name="Threshold/ Trigger" queryTableFieldId="17" dataDxfId="2"/>
+    <tableColumn id="19" uniqueName="Contingency_x005f_x0020_Start_x005f_x0020_Da" name="Contingency Start Date" queryTableFieldId="18" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1434,88 +1446,90 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="15" width="26.88671875" customWidth="1"/>
-    <col min="16" max="16" width="30.44140625" customWidth="1"/>
-    <col min="17" max="17" width="10.6640625" customWidth="1"/>
-    <col min="18" max="18" width="12.109375" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" customWidth="1"/>
-    <col min="21" max="21" width="25.6640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" customWidth="1"/>
+    <col min="17" max="17" width="30.42578125" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" customWidth="1"/>
+    <col min="20" max="20" width="20.7109375" customWidth="1"/>
+    <col min="21" max="21" width="15.28515625" customWidth="1"/>
+    <col min="22" max="22" width="25.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="24" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:22" ht="24" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="24"/>
-    </row>
-    <row r="2" spans="1:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="26"/>
+    </row>
+    <row r="2" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="27"/>
-    </row>
-    <row r="3" spans="1:21" ht="58.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="29"/>
+    </row>
+    <row r="3" spans="1:22" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1529,58 +1543,61 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="113.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="113.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
@@ -1591,57 +1608,58 @@
       <c r="D4" s="7">
         <v>40721</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="H4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="28">
+      <c r="K4" s="22">
         <v>1</v>
       </c>
-      <c r="K4" s="19">
+      <c r="L4" s="19">
         <v>5</v>
       </c>
-      <c r="L4" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="20">
+      <c r="M4" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="20">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
 Rating   (1-5)]]*5</f>
         <v>25</v>
       </c>
-      <c r="N4" s="10" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="5" t="s">
+      <c r="O4" s="10" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="R4" s="7">
         <v>41731</v>
       </c>
-      <c r="R4" s="7"/>
-      <c r="S4" s="5" t="s">
+      <c r="S4" s="7"/>
+      <c r="T4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="U4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="U4" s="7"/>
-    </row>
-    <row r="5" spans="1:21" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V4" s="7"/>
+    </row>
+    <row r="5" spans="1:22" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>49</v>
       </c>
@@ -1652,55 +1670,56 @@
       <c r="D5" s="7">
         <v>41013</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="7"/>
+      <c r="F5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="H5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="28">
+      <c r="K5" s="22">
         <v>1</v>
       </c>
-      <c r="K5" s="19">
+      <c r="L5" s="19">
         <v>1</v>
       </c>
-      <c r="L5" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="20">
+      <c r="M5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="20">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
 Rating   (1-5)]]*5</f>
         <v>5</v>
       </c>
-      <c r="N5" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O5" s="11"/>
-      <c r="P5" s="5" t="s">
+      <c r="O5" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
-      <c r="S5" s="5" t="s">
+      <c r="S5" s="7"/>
+      <c r="T5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="U5" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="T5" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="U5" s="7"/>
-    </row>
-    <row r="6" spans="1:21" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V5" s="7"/>
+    </row>
+    <row r="6" spans="1:22" ht="82.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
@@ -1711,118 +1730,122 @@
       <c r="D6" s="7">
         <v>41108</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="28">
+      <c r="K6" s="22">
         <v>1</v>
       </c>
-      <c r="K6" s="19">
+      <c r="L6" s="19">
         <v>1</v>
       </c>
-      <c r="L6" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="20">
+      <c r="M6" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="20">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
 Rating   (1-5)]]*5</f>
         <v>5</v>
       </c>
-      <c r="N6" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O6" s="12"/>
-      <c r="P6" s="5" t="s">
+      <c r="O6" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="R6" s="7">
         <v>41731</v>
       </c>
-      <c r="R6" s="7"/>
-      <c r="S6" s="5" t="s">
+      <c r="S6" s="7"/>
+      <c r="T6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="T6" s="4" t="s">
+      <c r="U6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="U6" s="7"/>
-    </row>
-    <row r="7" spans="1:21" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V6" s="7"/>
+    </row>
+    <row r="7" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="9">
         <v>41414</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="9">
+        <v>42058</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="28">
+      <c r="K7" s="22">
         <v>1</v>
       </c>
-      <c r="K7" s="19">
+      <c r="L7" s="19">
         <v>5</v>
       </c>
-      <c r="L7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="20">
+      <c r="M7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="20">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
 Rating   (1-5)]]*5</f>
         <v>25</v>
       </c>
-      <c r="N7" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O7" s="13"/>
-      <c r="P7" s="5" t="s">
+      <c r="O7" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="R7" s="9">
         <v>41760</v>
       </c>
-      <c r="R7" s="9"/>
-      <c r="S7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="T7" s="4" t="s">
+      <c r="S7" s="9"/>
+      <c r="T7" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="U7" s="9"/>
-    </row>
-    <row r="8" spans="1:21" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="V7" s="9"/>
+    </row>
+    <row r="8" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>24</v>
       </c>
@@ -1833,57 +1856,58 @@
       <c r="D8" s="9">
         <v>41438</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="28">
+      <c r="K8" s="22">
         <v>1</v>
       </c>
-      <c r="K8" s="19">
+      <c r="L8" s="19">
         <v>2</v>
       </c>
-      <c r="L8" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="20">
+      <c r="M8" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="20">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
 Rating   (1-5)]]*5</f>
         <v>10</v>
       </c>
-      <c r="N8" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O8" s="14"/>
-      <c r="P8" s="5" t="s">
+      <c r="O8" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="R8" s="9">
         <v>41791</v>
       </c>
-      <c r="R8" s="9"/>
-      <c r="S8" s="5" t="s">
+      <c r="S8" s="9"/>
+      <c r="T8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="U8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="T8" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="U8" s="9"/>
-    </row>
-    <row r="9" spans="1:21" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V8" s="9"/>
+    </row>
+    <row r="9" spans="1:22" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>49</v>
       </c>
@@ -1894,1137 +1918,1174 @@
       <c r="D9" s="9">
         <v>41619</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="9">
+        <v>41850</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="J9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="28">
+      <c r="K9" s="22">
         <v>0.25</v>
       </c>
-      <c r="K9" s="19">
+      <c r="L9" s="19">
         <v>4</v>
       </c>
-      <c r="L9" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="20">
+      <c r="M9" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="20">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
 Rating   (1-5)]]*5</f>
         <v>5</v>
       </c>
-      <c r="N9" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O9" s="15"/>
-      <c r="P9" s="5" t="s">
+      <c r="O9" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="R9" s="9">
         <v>41803</v>
       </c>
-      <c r="R9" s="9">
+      <c r="S9" s="9">
         <v>41850</v>
       </c>
-      <c r="S9" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="T9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="U9" s="9"/>
-    </row>
-    <row r="10" spans="1:21" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="T9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="V9" s="9"/>
+    </row>
+    <row r="10" spans="1:22" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="9">
         <v>41837</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="9">
+        <v>42058</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="28">
+      <c r="K10" s="22">
         <v>0.75</v>
       </c>
-      <c r="K10" s="19">
+      <c r="L10" s="19">
         <v>5</v>
       </c>
-      <c r="L10" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="20">
+      <c r="M10" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="20">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
 Rating   (1-5)]]*5</f>
         <v>18.75</v>
       </c>
-      <c r="N10" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O10" s="15"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="9"/>
+      <c r="O10" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="5"/>
       <c r="R10" s="9"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="9"/>
-    </row>
-    <row r="11" spans="1:21" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S10" s="9"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="V10" s="9"/>
+    </row>
+    <row r="11" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="9">
         <v>41850</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="9">
+        <v>42058</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="J11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="22">
+        <v>0.85</v>
+      </c>
+      <c r="L11" s="19">
+        <v>5</v>
+      </c>
+      <c r="M11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="20">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>21.25</v>
+      </c>
+      <c r="O11" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="R11" s="9">
+        <v>41850</v>
+      </c>
+      <c r="S11" s="9"/>
+      <c r="T11" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="28">
-        <v>0.85</v>
-      </c>
-      <c r="K11" s="19">
-        <v>5</v>
-      </c>
-      <c r="L11" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="20">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>21.25</v>
-      </c>
-      <c r="N11" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O11" s="15"/>
-      <c r="P11" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q11" s="9">
-        <v>41850</v>
-      </c>
-      <c r="R11" s="9"/>
-      <c r="S11" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="T11" s="8"/>
-      <c r="U11" s="9"/>
-    </row>
-    <row r="12" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U11" s="8"/>
+      <c r="V11" s="9"/>
+    </row>
+    <row r="12" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="4"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="4"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N12" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O12" s="15"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="9"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O12" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="5"/>
       <c r="R12" s="9"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="9"/>
-    </row>
-    <row r="13" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S12" s="9"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="9"/>
+    </row>
+    <row r="13" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="4"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N13" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O13" s="15"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="9"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O13" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="5"/>
       <c r="R13" s="9"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="9"/>
-    </row>
-    <row r="14" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S13" s="9"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="9"/>
+    </row>
+    <row r="14" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="4"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="4"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N14" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O14" s="15"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="9"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O14" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="5"/>
       <c r="R14" s="9"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="9"/>
-    </row>
-    <row r="15" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S14" s="9"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="9"/>
+    </row>
+    <row r="15" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="4"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="4"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N15" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O15" s="15"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="9"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O15" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="5"/>
       <c r="R15" s="9"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="9"/>
-    </row>
-    <row r="16" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S15" s="9"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="9"/>
+    </row>
+    <row r="16" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="4"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="4"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M16" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N16" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O16" s="15"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="9"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O16" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="5"/>
       <c r="R16" s="9"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="9"/>
-    </row>
-    <row r="17" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S16" s="9"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="9"/>
+    </row>
+    <row r="17" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="4"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="4"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L17" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N17" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O17" s="15"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="9"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O17" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="5"/>
       <c r="R17" s="9"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="9"/>
-    </row>
-    <row r="18" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S17" s="9"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="9"/>
+    </row>
+    <row r="18" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="4"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="4"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L18" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M18" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N18" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O18" s="15"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="9"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N18" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O18" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="5"/>
       <c r="R18" s="9"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="9"/>
-    </row>
-    <row r="19" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S18" s="9"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="9"/>
+    </row>
+    <row r="19" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="4"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="4"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M19" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N19" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O19" s="15"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="9"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N19" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O19" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="5"/>
       <c r="R19" s="9"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="9"/>
-    </row>
-    <row r="20" spans="1:21" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S19" s="9"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="9"/>
+    </row>
+    <row r="20" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="4"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="4"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N20" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O20" s="15"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="9"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O20" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="5"/>
       <c r="R20" s="9"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="9"/>
-    </row>
-    <row r="21" spans="1:21" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S20" s="9"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="9"/>
+    </row>
+    <row r="21" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="4"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="4"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M21" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N21" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O21" s="15"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="9"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O21" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="5"/>
       <c r="R21" s="9"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="9"/>
-    </row>
-    <row r="22" spans="1:21" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S21" s="9"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="9"/>
+    </row>
+    <row r="22" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="4"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="4"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L22" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N22" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O22" s="15"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="9"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N22" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O22" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="5"/>
       <c r="R22" s="9"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="9"/>
-    </row>
-    <row r="23" spans="1:21" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S22" s="9"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="9"/>
+    </row>
+    <row r="23" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="4"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="4"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M23" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N23" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O23" s="15"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="9"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N23" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O23" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="5"/>
       <c r="R23" s="9"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="9"/>
-    </row>
-    <row r="24" spans="1:21" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S23" s="9"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="9"/>
+    </row>
+    <row r="24" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="4"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="4"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L24" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M24" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N24" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O24" s="15"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="9"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M24" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N24" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O24" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="5"/>
       <c r="R24" s="9"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="9"/>
-    </row>
-    <row r="25" spans="1:21" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S24" s="9"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="9"/>
+    </row>
+    <row r="25" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="4"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="4"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L25" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M25" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N25" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O25" s="15"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="9"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M25" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N25" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O25" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="5"/>
       <c r="R25" s="9"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="9"/>
-    </row>
-    <row r="26" spans="1:21" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S25" s="9"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="9"/>
+    </row>
+    <row r="26" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="4"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="4"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L26" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M26" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N26" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O26" s="15"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="9"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M26" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N26" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O26" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="5"/>
       <c r="R26" s="9"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="9"/>
-    </row>
-    <row r="27" spans="1:21" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S26" s="9"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="9"/>
+    </row>
+    <row r="27" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="4"/>
       <c r="D27" s="9"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="4"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="5"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L27" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M27" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N27" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O27" s="15"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="9"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N27" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O27" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="5"/>
       <c r="R27" s="9"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="9"/>
-    </row>
-    <row r="28" spans="1:21" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S27" s="9"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="9"/>
+    </row>
+    <row r="28" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="4"/>
       <c r="D28" s="9"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="4"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K28" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L28" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M28" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N28" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O28" s="15"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="9"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M28" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O28" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="5"/>
       <c r="R28" s="9"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="9"/>
-    </row>
-    <row r="29" spans="1:21" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S28" s="9"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="9"/>
+    </row>
+    <row r="29" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="4"/>
       <c r="D29" s="9"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="4"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="5"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K29" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L29" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M29" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N29" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O29" s="15"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="9"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M29" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N29" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O29" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="5"/>
       <c r="R29" s="9"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="9"/>
-    </row>
-    <row r="30" spans="1:21" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S29" s="9"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="8"/>
+      <c r="V29" s="9"/>
+    </row>
+    <row r="30" spans="1:22" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="4"/>
       <c r="D30" s="9"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="4"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="5"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K30" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L30" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M30" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N30" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O30" s="15"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="9"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M30" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N30" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O30" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="5"/>
       <c r="R30" s="9"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="9"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S30" s="9"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="8"/>
+      <c r="V30" s="9"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="4"/>
       <c r="D31" s="9"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="4"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="5"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K31" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M31" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N31" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O31" s="15"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="9"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N31" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O31" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="5"/>
       <c r="R31" s="9"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="9"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S31" s="9"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="8"/>
+      <c r="V31" s="9"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="4"/>
       <c r="D32" s="9"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="4"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="5"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K32" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L32" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M32" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N32" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O32" s="15"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="9"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N32" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O32" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="5"/>
       <c r="R32" s="9"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="9"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S32" s="9"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="8"/>
+      <c r="V32" s="9"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="4"/>
       <c r="D33" s="9"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="4"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="5"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K33" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L33" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M33" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N33" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O33" s="15"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="9"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N33" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O33" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="5"/>
       <c r="R33" s="9"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="9"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S33" s="9"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="8"/>
+      <c r="V33" s="9"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="4"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="4"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="5"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K34" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L34" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M34" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N34" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O34" s="15"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="9"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N34" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O34" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="5"/>
       <c r="R34" s="9"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="9"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S34" s="9"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="9"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="4"/>
       <c r="D35" s="9"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="4"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="5"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K35" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L35" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M35" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N35" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O35" s="15"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="9"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M35" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N35" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O35" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="5"/>
       <c r="R35" s="9"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="9"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S35" s="9"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="8"/>
+      <c r="V35" s="9"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="4"/>
       <c r="D36" s="9"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="4"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="5"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K36" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L36" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M36" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N36" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O36" s="15"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="9"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L36" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M36" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N36" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O36" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="5"/>
       <c r="R36" s="9"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="9"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="S36" s="9"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="9"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="17"/>
       <c r="D37" s="9"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="4"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="5"/>
       <c r="G37" s="4"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K37" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L37" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="M37" s="20" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
-Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N37" s="11" t="e">
-        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
-$]]</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O37" s="16"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="9"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="L37" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M37" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N37" s="20" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
+Rating   (1-5)]]*5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O37" s="11" t="e">
+        <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
+$]]</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="5"/>
       <c r="R37" s="9"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="5"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:U2"/>
+    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="A2:V2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="17" scale="38" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="17" scale="36" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;LVangent Proprietary Information</oddFooter>
   </headerFooter>
@@ -3035,18 +3096,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3164,6 +3225,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -3174,14 +3243,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[VM:timothy.queen@3/6/2015 10:29:14 AM] updated
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13968
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
+++ b/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="75">
   <si>
     <t>Status</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Provide training for users. Ensure that the message is reinforced through coaching. Provide SOPs for users</t>
   </si>
   <si>
-    <t>Incomplete and inaccurate data in centralized CCO CSR/Employee database (eWFM/roster raw) - creates inconsistencies in records being created from external sources (quality control system) compated to records created directly in eCL.</t>
-  </si>
-  <si>
     <t>Incomplete and inaccurate data in centrallized CCO CSR/Employee database</t>
   </si>
   <si>
@@ -246,6 +243,18 @@
   </si>
   <si>
     <t>Monitoring system changes; Verint went into production July 1, 2014; closed 2/23/15</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
+    <t>Incomplete and inaccurate data in centralized CCO CSR/Employee database (eWFM/roster raw) - creates inconsistencies in records being created from external sources (quality control system) compared to records created directly in eCL.</t>
+  </si>
+  <si>
+    <t>access to warning information</t>
   </si>
 </sst>
 </file>
@@ -962,10 +971,6 @@
   <dxfs count="23">
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1059,6 +1064,10 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1125,32 +1134,40 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_owssvr_23" displayName="Table_owssvr_23" ref="A3:V37" tableType="queryTable" totalsRowShown="0" dataDxfId="22">
+  <autoFilter ref="A3:V37">
+    <filterColumn colId="0">
+      <filters blank="1">
+        <filter val="new"/>
+        <filter val="open"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="22">
     <tableColumn id="1" uniqueName="Status" name="Status" queryTableFieldId="2" dataDxfId="21"/>
     <tableColumn id="2" uniqueName="Project" name="Program" queryTableFieldId="20" dataDxfId="20"/>
     <tableColumn id="3" uniqueName="Title" name="Risk Description" queryTableFieldId="1" dataDxfId="19"/>
     <tableColumn id="4" uniqueName="Date_x005f_x0020_Identified" name="Date Identified" queryTableFieldId="3" dataDxfId="18"/>
-    <tableColumn id="23" uniqueName="23" name="Date Modified" queryTableFieldId="27" dataDxfId="0"/>
-    <tableColumn id="5" uniqueName="Context" name="Context" queryTableFieldId="4" dataDxfId="17"/>
-    <tableColumn id="6" uniqueName="Owner" name="Risk Owner" queryTableFieldId="5" dataDxfId="16"/>
-    <tableColumn id="7" uniqueName="Origin" name="Origin" queryTableFieldId="6" dataDxfId="15"/>
-    <tableColumn id="8" uniqueName="Stakeholders" name="Stakeholders" queryTableFieldId="7" dataDxfId="14"/>
-    <tableColumn id="9" uniqueName="Category" name="Category" queryTableFieldId="8" dataDxfId="13"/>
-    <tableColumn id="10" uniqueName="Probability" name="Probability of Occurrence (%) " queryTableFieldId="9" dataDxfId="12" dataCellStyle="Percent"/>
-    <tableColumn id="11" uniqueName="Impact" name="Impact  _x000a_Rating   (1-5)" queryTableFieldId="10" dataDxfId="11" dataCellStyle="Currency"/>
-    <tableColumn id="21" uniqueName="21" name="Total Impact on occurance_x000a_$" queryTableFieldId="26" dataDxfId="10" dataCellStyle="Currency"/>
-    <tableColumn id="12" uniqueName="Risk_x005f_x0020_Exposure" name="Risk Exposure Ranking_x000a_(1 - 25)" queryTableFieldId="11" dataDxfId="9"/>
-    <tableColumn id="13" uniqueName="13" name="Risk Exposure Estimate   ($)" queryTableFieldId="24" dataDxfId="8">
+    <tableColumn id="23" uniqueName="23" name="Date Modified" queryTableFieldId="27" dataDxfId="17"/>
+    <tableColumn id="5" uniqueName="Context" name="Context" queryTableFieldId="4" dataDxfId="16"/>
+    <tableColumn id="6" uniqueName="Owner" name="Risk Owner" queryTableFieldId="5" dataDxfId="15"/>
+    <tableColumn id="7" uniqueName="Origin" name="Origin" queryTableFieldId="6" dataDxfId="14"/>
+    <tableColumn id="8" uniqueName="Stakeholders" name="Stakeholders" queryTableFieldId="7" dataDxfId="13"/>
+    <tableColumn id="9" uniqueName="Category" name="Category" queryTableFieldId="8" dataDxfId="12"/>
+    <tableColumn id="10" uniqueName="Probability" name="Probability of Occurrence (%) " queryTableFieldId="9" dataDxfId="11" dataCellStyle="Percent"/>
+    <tableColumn id="11" uniqueName="Impact" name="Impact  _x000a_Rating   (1-5)" queryTableFieldId="10" dataDxfId="10" dataCellStyle="Currency"/>
+    <tableColumn id="21" uniqueName="21" name="Total Impact on occurance_x000a_$" queryTableFieldId="26" dataDxfId="9" dataCellStyle="Currency"/>
+    <tableColumn id="12" uniqueName="Risk_x005f_x0020_Exposure" name="Risk Exposure Ranking_x000a_(1 - 25)" queryTableFieldId="11" dataDxfId="8"/>
+    <tableColumn id="13" uniqueName="13" name="Risk Exposure Estimate   ($)" queryTableFieldId="24" dataDxfId="7">
       <calculatedColumnFormula>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
 $]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" uniqueName="20" name="Basis of Risk Exposure Estimate" queryTableFieldId="25" dataDxfId="7"/>
-    <tableColumn id="14" uniqueName="Mitigation_x005f_x0020_Plan" name="Mitigation Plan" queryTableFieldId="13" dataDxfId="6"/>
-    <tableColumn id="15" uniqueName="Mitigation_x005f_x0020_Start_x005f_x0020_Dat" name="Mitigation Start Date" queryTableFieldId="14" dataDxfId="5"/>
-    <tableColumn id="16" uniqueName="Mitigation_x005f_x0020_Stop_x005f_x0020_Date" name="Mitigation Stop Date" queryTableFieldId="15" dataDxfId="4"/>
-    <tableColumn id="17" uniqueName="Contingency_x005f_x0020_Plan" name="Contingency Plan" queryTableFieldId="16" dataDxfId="3"/>
-    <tableColumn id="18" uniqueName="Threshold_x005f_x002f_Trigger" name="Threshold/ Trigger" queryTableFieldId="17" dataDxfId="2"/>
-    <tableColumn id="19" uniqueName="Contingency_x005f_x0020_Start_x005f_x0020_Da" name="Contingency Start Date" queryTableFieldId="18" dataDxfId="1"/>
+    <tableColumn id="20" uniqueName="20" name="Basis of Risk Exposure Estimate" queryTableFieldId="25" dataDxfId="6"/>
+    <tableColumn id="14" uniqueName="Mitigation_x005f_x0020_Plan" name="Mitigation Plan" queryTableFieldId="13" dataDxfId="5"/>
+    <tableColumn id="15" uniqueName="Mitigation_x005f_x0020_Start_x005f_x0020_Dat" name="Mitigation Start Date" queryTableFieldId="14" dataDxfId="4"/>
+    <tableColumn id="16" uniqueName="Mitigation_x005f_x0020_Stop_x005f_x0020_Date" name="Mitigation Stop Date" queryTableFieldId="15" dataDxfId="3"/>
+    <tableColumn id="17" uniqueName="Contingency_x005f_x0020_Plan" name="Contingency Plan" queryTableFieldId="16" dataDxfId="2"/>
+    <tableColumn id="18" uniqueName="Threshold_x005f_x002f_Trigger" name="Threshold/ Trigger" queryTableFieldId="17" dataDxfId="1"/>
+    <tableColumn id="19" uniqueName="Contingency_x005f_x0020_Start_x005f_x0020_Da" name="Contingency Start Date" queryTableFieldId="18" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1448,8 +1465,8 @@
   </sheetPr>
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,7 +1560,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>2</v>
@@ -1599,7 +1616,7 @@
     </row>
     <row r="4" spans="1:22" ht="113.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="4" t="s">
@@ -1608,7 +1625,9 @@
       <c r="D4" s="7">
         <v>40721</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="9">
+        <v>42060</v>
+      </c>
       <c r="F4" s="5" t="s">
         <v>26</v>
       </c>
@@ -1652,16 +1671,16 @@
       </c>
       <c r="S4" s="7"/>
       <c r="T4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U4" s="8" t="s">
         <v>31</v>
       </c>
       <c r="V4" s="7"/>
     </row>
-    <row r="5" spans="1:22" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="66.599999999999994" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="4" t="s">
@@ -1672,7 +1691,7 @@
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>33</v>
@@ -1712,10 +1731,10 @@
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="U5" s="8" t="s">
         <v>56</v>
-      </c>
-      <c r="U5" s="8" t="s">
-        <v>57</v>
       </c>
       <c r="V5" s="7"/>
     </row>
@@ -1725,14 +1744,14 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="4" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="D6" s="7">
         <v>41108</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>33</v>
@@ -1767,27 +1786,27 @@
       </c>
       <c r="P6" s="12"/>
       <c r="Q6" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R6" s="7">
         <v>41731</v>
       </c>
       <c r="S6" s="7"/>
       <c r="T6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="U6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="U6" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="V6" s="7"/>
     </row>
-    <row r="7" spans="1:22" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="63" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="9">
         <v>41414</v>
@@ -1796,7 +1815,7 @@
         <v>42058</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>33</v>
@@ -1831,34 +1850,36 @@
       </c>
       <c r="P7" s="13"/>
       <c r="Q7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R7" s="9">
         <v>41760</v>
       </c>
       <c r="S7" s="9"/>
       <c r="T7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="V7" s="9"/>
     </row>
     <row r="8" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="9">
         <v>41438</v>
       </c>
-      <c r="E8" s="9"/>
+      <c r="E8" s="9">
+        <v>42060</v>
+      </c>
       <c r="F8" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>33</v>
@@ -1893,27 +1914,27 @@
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R8" s="9">
         <v>41791</v>
       </c>
       <c r="S8" s="9"/>
       <c r="T8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U8" s="8" t="s">
-        <v>54</v>
-      </c>
       <c r="V8" s="9"/>
     </row>
-    <row r="9" spans="1:22" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="88.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="9">
         <v>41619</v>
@@ -1922,7 +1943,7 @@
         <v>41850</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>33</v>
@@ -1957,7 +1978,7 @@
       </c>
       <c r="P9" s="15"/>
       <c r="Q9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R9" s="9">
         <v>41803</v>
@@ -1966,20 +1987,20 @@
         <v>41850</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V9" s="9"/>
     </row>
-    <row r="10" spans="1:22" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="57.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="9">
         <v>41837</v>
@@ -1988,14 +2009,14 @@
         <v>42058</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>34</v>
@@ -2025,7 +2046,7 @@
       <c r="S10" s="9"/>
       <c r="T10" s="5"/>
       <c r="U10" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V10" s="9"/>
     </row>
@@ -2035,7 +2056,7 @@
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="9">
         <v>41850</v>
@@ -2044,16 +2065,16 @@
         <v>42058</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>29</v>
@@ -2079,23 +2100,29 @@
       </c>
       <c r="P11" s="15"/>
       <c r="Q11" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R11" s="9">
         <v>41850</v>
       </c>
       <c r="S11" s="9"/>
       <c r="T11" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U11" s="8"/>
       <c r="V11" s="9"/>
     </row>
     <row r="12" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="9"/>
+      <c r="C12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="9">
+        <v>42060</v>
+      </c>
       <c r="E12" s="9"/>
       <c r="F12" s="5"/>
       <c r="G12" s="4"/>
@@ -2130,7 +2157,9 @@
       <c r="V12" s="9"/>
     </row>
     <row r="13" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="B13" s="8"/>
       <c r="C13" s="4"/>
       <c r="D13" s="9"/>
@@ -2168,7 +2197,9 @@
       <c r="V13" s="9"/>
     </row>
     <row r="14" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="B14" s="8"/>
       <c r="C14" s="4"/>
       <c r="D14" s="9"/>
@@ -2206,7 +2237,9 @@
       <c r="V14" s="9"/>
     </row>
     <row r="15" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="8" t="s">
+        <v>71</v>
+      </c>
       <c r="B15" s="8"/>
       <c r="C15" s="4"/>
       <c r="D15" s="9"/>
@@ -3096,18 +3129,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3225,14 +3258,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -3243,6 +3268,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[VM:timothy.queen@3/25/2015 1:47:08 PM] updated risks
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C13982
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
+++ b/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="81">
   <si>
     <t>Status</t>
   </si>
@@ -255,6 +255,24 @@
   </si>
   <si>
     <t>access to warning information</t>
+  </si>
+  <si>
+    <t>Access to warnings must be limited to specific individuals</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Access is controlled through an access control list, supervisors and managers</t>
+  </si>
+  <si>
+    <t>Ensure all staff on the project understand the sensitivity of the data</t>
+  </si>
+  <si>
+    <t>Exposure</t>
+  </si>
+  <si>
+    <t>individuals identified in OY3 will be more aligned with the project</t>
   </si>
 </sst>
 </file>
@@ -1465,8 +1483,8 @@
   </sheetPr>
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,7 +1632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="113.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="113.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>72</v>
       </c>
@@ -1864,7 +1882,7 @@
       </c>
       <c r="V7" s="9"/>
     </row>
-    <row r="8" spans="1:22" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="66" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>72</v>
       </c>
@@ -2062,7 +2080,7 @@
         <v>41850</v>
       </c>
       <c r="E11" s="9">
-        <v>42058</v>
+        <v>42088</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>69</v>
@@ -2107,7 +2125,7 @@
       </c>
       <c r="S11" s="9"/>
       <c r="T11" s="5" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="U11" s="8"/>
       <c r="V11" s="9"/>
@@ -2123,25 +2141,37 @@
       <c r="D12" s="9">
         <v>42060</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="19" t="s">
-        <v>21</v>
+      <c r="E12" s="9">
+        <v>42088</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="L12" s="19">
+        <v>3</v>
       </c>
       <c r="M12" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="20" t="e">
+      <c r="N12" s="20">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
 Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
+        <v>3.0000000000000004</v>
       </c>
       <c r="O12" s="11" t="e">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
@@ -2149,11 +2179,19 @@
         <v>#VALUE!</v>
       </c>
       <c r="P12" s="15"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="9"/>
+      <c r="Q12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="R12" s="9">
+        <v>42064</v>
+      </c>
       <c r="S12" s="9"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="8"/>
+      <c r="T12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="U12" s="8" t="s">
+        <v>79</v>
+      </c>
       <c r="V12" s="9"/>
     </row>
     <row r="13" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -3129,18 +3167,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3258,6 +3296,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -3268,14 +3314,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[VM:timothy.queen@4/2/2015 10:41:48 AM] updated with review history
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C14006
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
+++ b/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7485"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Integrated Register" sheetId="2" r:id="rId1"/>
+    <sheet name="Review History" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="owssvr_2" localSheetId="0" hidden="1">'Integrated Register'!$A$3:$V$37</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="84">
   <si>
     <t>Status</t>
   </si>
@@ -273,6 +274,15 @@
   </si>
   <si>
     <t>individuals identified in OY3 will be more aligned with the project</t>
+  </si>
+  <si>
+    <t>added risk on warnings</t>
+  </si>
+  <si>
+    <t>Updated mitigation on warnings</t>
+  </si>
+  <si>
+    <t>Review of risks with Team  no updates</t>
   </si>
 </sst>
 </file>
@@ -850,7 +860,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -939,6 +949,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1483,8 +1494,8 @@
   </sheetPr>
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3166,19 +3177,61 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="30">
+        <v>42060</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="30">
+        <v>42088</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="30">
+        <v>42096</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3296,14 +3349,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -3314,6 +3359,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
[VM:timothy.queen@5/13/2015 1:53:46 PM] Risk review for May; closed one risk add two more.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C14092
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
+++ b/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="13395" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="Integrated Register" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="90">
   <si>
     <t>Status</t>
   </si>
@@ -283,6 +283,24 @@
   </si>
   <si>
     <t>Review of risks with Team  no updates</t>
+  </si>
+  <si>
+    <t>SMTP server may not working for production</t>
+  </si>
+  <si>
+    <t>Notifications will not get sent out.</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>File share access changing without warning</t>
+  </si>
+  <si>
+    <t>Application will not work</t>
+  </si>
+  <si>
+    <t>Closed row 12; added two new risks</t>
   </si>
 </sst>
 </file>
@@ -931,6 +949,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -949,7 +968,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1494,8 +1512,8 @@
   </sheetPr>
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,56 +1542,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="24" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="27"/>
     </row>
     <row r="2" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="30"/>
     </row>
     <row r="3" spans="1:22" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2143,7 +2161,7 @@
     </row>
     <row r="12" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="4" t="s">
@@ -2153,7 +2171,7 @@
         <v>42060</v>
       </c>
       <c r="E12" s="9">
-        <v>42088</v>
+        <v>42137</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>75</v>
@@ -2207,13 +2225,19 @@
     </row>
     <row r="13" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="9"/>
+      <c r="C13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="9">
+        <v>42137</v>
+      </c>
       <c r="E13" s="9"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -2247,13 +2271,19 @@
     </row>
     <row r="14" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="B14" s="8"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="9"/>
+      <c r="C14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="9">
+        <v>42137</v>
+      </c>
       <c r="E14" s="9"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -3179,10 +3209,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3191,7 +3221,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="30">
+      <c r="A1" s="24">
         <v>42060</v>
       </c>
       <c r="B1" t="s">
@@ -3199,7 +3229,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="30">
+      <c r="A2" s="24">
         <v>42088</v>
       </c>
       <c r="B2" t="s">
@@ -3207,11 +3237,19 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="30">
+      <c r="A3" s="24">
         <v>42096</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="24">
+        <v>42137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3226,15 +3264,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E5C6E04F5F2CA4DBF07DC2DA055DA5A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b67af60ff7fc8b8e5184fdb460baaf96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -3348,6 +3377,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
@@ -3364,14 +3402,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9FB9A1-B4D8-4EF0-9C41-8E101BF6B1F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3385,4 +3415,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated during 7/8 meeting
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C32476
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
+++ b/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="92">
   <si>
     <t>Status</t>
   </si>
@@ -301,6 +301,12 @@
   </si>
   <si>
     <t>Closed row 12; added two new risks</t>
+  </si>
+  <si>
+    <t>Jourdain</t>
+  </si>
+  <si>
+    <t>Coaching logs are being entered with PII</t>
   </si>
 </sst>
 </file>
@@ -1512,8 +1518,8 @@
   </sheetPr>
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2238,23 +2244,31 @@
       <c r="F13" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="19" t="s">
-        <v>21</v>
+      <c r="G13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="L13" s="19">
+        <v>2</v>
       </c>
       <c r="M13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="N13" s="20" t="e">
+      <c r="N13" s="20">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
 Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="O13" s="11" t="e">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
@@ -2284,23 +2298,31 @@
       <c r="F14" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="L14" s="19" t="s">
-        <v>21</v>
+      <c r="G14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="L14" s="19">
+        <v>2</v>
       </c>
       <c r="M14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="N14" s="20" t="e">
+      <c r="N14" s="20">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Impact  
 Rating   (1-5)]]*5</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="O14" s="11" t="e">
         <f>Table_owssvr_23[[#This Row],[Probability of Occurrence (%) ]]*Table_owssvr_23[[#This Row],[Total Impact on occurance
@@ -2320,7 +2342,9 @@
         <v>71</v>
       </c>
       <c r="B15" s="8"/>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="5"/>
@@ -3264,6 +3288,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E5C6E04F5F2CA4DBF07DC2DA055DA5A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b67af60ff7fc8b8e5184fdb460baaf96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -3377,15 +3410,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
@@ -3402,6 +3426,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9FB9A1-B4D8-4EF0-9C41-8E101BF6B1F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3415,12 +3447,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated during eCL weekly meeting.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C32818
</commit_message>
<xml_diff>
--- a/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
+++ b/Project Management/CCO OY2_eCoaching Log Risk Register.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="91">
   <si>
     <t>Status</t>
   </si>
@@ -244,9 +244,6 @@
   </si>
   <si>
     <t>Monitoring system changes; Verint went into production July 1, 2014; closed 2/23/15</t>
-  </si>
-  <si>
-    <t>new</t>
   </si>
   <si>
     <t>closed</t>
@@ -1518,8 +1515,8 @@
   </sheetPr>
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1666,7 @@
     </row>
     <row r="4" spans="1:22" ht="113.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="4" t="s">
@@ -1797,7 +1794,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="7">
         <v>41108</v>
@@ -1919,7 +1916,7 @@
     </row>
     <row r="8" spans="1:22" ht="66" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="4" t="s">
@@ -2160,7 +2157,7 @@
       </c>
       <c r="S11" s="9"/>
       <c r="T11" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U11" s="8"/>
       <c r="V11" s="9"/>
@@ -2171,7 +2168,7 @@
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="9">
         <v>42060</v>
@@ -2180,10 +2177,10 @@
         <v>42137</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>27</v>
@@ -2215,34 +2212,36 @@
       </c>
       <c r="P12" s="15"/>
       <c r="Q12" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R12" s="9">
         <v>42064</v>
       </c>
       <c r="S12" s="9"/>
       <c r="T12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="U12" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="U12" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="V12" s="9"/>
     </row>
     <row r="13" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="9">
         <v>42137</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="9">
+        <v>42242</v>
+      </c>
       <c r="F13" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>64</v>
@@ -2285,24 +2284,24 @@
     </row>
     <row r="14" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="9">
         <v>42137</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>64</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>65</v>
@@ -2339,13 +2338,15 @@
     </row>
     <row r="15" spans="1:22" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D15" s="9"/>
+        <v>90</v>
+      </c>
+      <c r="D15" s="9">
+        <v>42137</v>
+      </c>
       <c r="E15" s="9"/>
       <c r="F15" s="5"/>
       <c r="G15" s="4"/>
@@ -3249,7 +3250,7 @@
         <v>42060</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3257,7 +3258,7 @@
         <v>42088</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3265,7 +3266,7 @@
         <v>42096</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3273,7 +3274,7 @@
         <v>42137</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -3288,15 +3289,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E5C6E04F5F2CA4DBF07DC2DA055DA5A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b67af60ff7fc8b8e5184fdb460baaf96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -3410,6 +3402,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{137DE3B9-4E89-4FE7-800F-7F9802FB0CC4}">
   <ds:schemaRefs>
@@ -3426,14 +3427,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE9FB9A1-B4D8-4EF0-9C41-8E101BF6B1F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3447,4 +3440,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347E97F-5AA5-4FD3-B7C6-A3BFBE262F09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>